<commit_message>
Completed varying queue size tests
</commit_message>
<xml_diff>
--- a/Tests/Set 11 [Varied Queue Size]/Combined Varied Queue Size Test Summary.xlsx
+++ b/Tests/Set 11 [Varied Queue Size]/Combined Varied Queue Size Test Summary.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE5A71D-B25C-4A96-A799-BA20526E01F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01384285-614E-4A5B-AA72-4DD576330AC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Varied Queue Size Tests</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>Number of Measurements</t>
+  </si>
+  <si>
+    <t>4 hours 17 mins</t>
   </si>
 </sst>
 </file>
@@ -157,7 +160,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -279,11 +282,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -373,6 +385,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -655,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:I19"/>
+  <dimension ref="B2:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +689,7 @@
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -698,7 +713,7 @@
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -708,7 +723,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -718,38 +733,43 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>10</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="5">
+      <c r="F5" s="5">
         <v>100</v>
       </c>
-      <c r="E5" s="4">
+      <c r="G5" s="4">
         <v>500</v>
       </c>
-      <c r="F5" s="18">
+      <c r="H5" s="18">
         <v>1000</v>
       </c>
-      <c r="G5" s="4">
+      <c r="I5" s="4">
         <v>10000</v>
       </c>
-      <c r="H5" s="19">
+      <c r="J5" s="19">
         <v>100000</v>
       </c>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="6">
         <v>1000</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="31">
         <v>1000</v>
       </c>
       <c r="E6" s="8">
@@ -761,96 +781,118 @@
       <c r="G6" s="8">
         <v>1000</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="7">
+        <v>1000</v>
+      </c>
+      <c r="I6" s="8">
+        <v>1000</v>
+      </c>
+      <c r="J6" s="9">
         <v>955</v>
       </c>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="11">
+        <v>8039</v>
+      </c>
+      <c r="D7" s="8">
+        <v>337</v>
+      </c>
+      <c r="E7" s="12">
         <v>966059</v>
       </c>
-      <c r="D7" s="8">
+      <c r="F7" s="8">
         <v>974.2</v>
       </c>
-      <c r="E7" s="12">
+      <c r="G7" s="12">
         <v>5075.5</v>
       </c>
-      <c r="F7" s="8">
+      <c r="H7" s="8">
         <v>9371.5</v>
       </c>
-      <c r="G7" s="12">
+      <c r="I7" s="12">
         <v>103811</v>
       </c>
-      <c r="H7" s="13">
+      <c r="J7" s="13">
         <v>1079720</v>
       </c>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="D8" s="7">
+        <v>16</v>
+      </c>
+      <c r="E8" s="8">
         <v>8.6999999999999993</v>
       </c>
-      <c r="D8" s="7">
+      <c r="F8" s="7">
         <v>40.200000000000003</v>
       </c>
-      <c r="E8" s="8">
+      <c r="G8" s="8">
         <v>33.299999999999997</v>
       </c>
-      <c r="F8" s="7">
+      <c r="H8" s="7">
         <v>37.6</v>
       </c>
-      <c r="G8" s="8">
+      <c r="I8" s="8">
         <v>38</v>
       </c>
-      <c r="H8" s="9">
+      <c r="J8" s="9">
         <v>34.9</v>
       </c>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="14">
+        <v>15426</v>
+      </c>
+      <c r="D9" s="15">
+        <v>49</v>
+      </c>
+      <c r="E9" s="16">
         <v>37431</v>
       </c>
-      <c r="D9" s="15">
+      <c r="F9" s="15">
         <v>19</v>
       </c>
-      <c r="E9" s="16">
+      <c r="G9" s="16">
         <v>21</v>
       </c>
-      <c r="F9" s="15">
+      <c r="H9" s="15">
         <v>18</v>
       </c>
-      <c r="G9" s="16">
+      <c r="I9" s="16">
         <v>19</v>
       </c>
-      <c r="H9" s="17">
+      <c r="J9" s="17">
         <v>20</v>
       </c>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-    </row>
-    <row r="13" spans="2:9" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="J10" s="3"/>
+    </row>
+    <row r="13" spans="2:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B13" s="21" t="s">
         <v>0</v>
       </c>
@@ -868,95 +910,119 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="22" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="23">
+        <v>1</v>
+      </c>
+      <c r="D16" s="23">
+        <v>10</v>
+      </c>
+      <c r="E16" s="23">
         <v>50</v>
       </c>
-      <c r="D16" s="23">
+      <c r="F16" s="23">
         <v>100</v>
       </c>
-      <c r="E16" s="23">
+      <c r="G16" s="23">
         <v>500</v>
       </c>
-      <c r="F16" s="23">
+      <c r="H16" s="23">
         <v>1000</v>
       </c>
-      <c r="G16" s="23">
+      <c r="I16" s="23">
         <v>10000</v>
       </c>
-      <c r="H16" s="24">
+      <c r="J16" s="24">
         <v>100000</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="26">
+        <v>5</v>
+      </c>
+      <c r="D17" s="26">
+        <v>5</v>
+      </c>
+      <c r="E17" s="26">
         <v>2</v>
       </c>
-      <c r="D17" s="26">
+      <c r="F17" s="26">
         <v>4</v>
       </c>
-      <c r="E17" s="26">
+      <c r="G17" s="26">
         <v>5</v>
       </c>
-      <c r="F17" s="26">
+      <c r="H17" s="26">
         <v>3</v>
       </c>
-      <c r="G17" s="26">
+      <c r="I17" s="26">
         <v>3</v>
       </c>
-      <c r="H17" s="27">
+      <c r="J17" s="27">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="22" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="23">
+        <v>2965285</v>
+      </c>
+      <c r="D18" s="23">
+        <v>3007046</v>
+      </c>
+      <c r="E18" s="23">
         <v>4984</v>
       </c>
-      <c r="D18" s="23">
+      <c r="F18" s="23">
         <v>2878</v>
       </c>
-      <c r="E18" s="23">
+      <c r="G18" s="23">
         <v>2127</v>
       </c>
-      <c r="F18" s="23">
+      <c r="H18" s="23">
         <v>4820</v>
       </c>
-      <c r="G18" s="23">
+      <c r="I18" s="23">
         <v>2816</v>
       </c>
-      <c r="H18" s="24">
+      <c r="J18" s="24">
         <v>2420</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="28" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="29">
+        <v>79</v>
+      </c>
+      <c r="D19" s="29">
+        <v>77</v>
+      </c>
+      <c r="E19" s="29">
         <v>1.2</v>
       </c>
-      <c r="D19" s="29">
+      <c r="F19" s="29">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E19" s="29">
+      <c r="G19" s="29">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F19" s="29">
+      <c r="H19" s="29">
         <v>4.4000000000000004</v>
       </c>
-      <c r="G19" s="29">
+      <c r="I19" s="29">
         <v>3.9</v>
       </c>
-      <c r="H19" s="30">
+      <c r="J19" s="30">
         <v>1.1000000000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added more tests for varying queue size
</commit_message>
<xml_diff>
--- a/Tests/Set 11 [Varied Queue Size]/Combined Varied Queue Size Test Summary.xlsx
+++ b/Tests/Set 11 [Varied Queue Size]/Combined Varied Queue Size Test Summary.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01384285-614E-4A5B-AA72-4DD576330AC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D262E13F-6D30-4B2A-8F8F-93DE8012DF06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23880" yWindow="1935" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>Varied Queue Size Tests</t>
   </si>
@@ -58,9 +58,6 @@
     <t>50 (40KB)</t>
   </si>
   <si>
-    <t>Keyed</t>
-  </si>
-  <si>
     <t>10 hours 24 mins</t>
   </si>
   <si>
@@ -74,6 +71,15 @@
   </si>
   <si>
     <t>4 hours 17 mins</t>
+  </si>
+  <si>
+    <t>Run 1</t>
+  </si>
+  <si>
+    <t>Run 2</t>
+  </si>
+  <si>
+    <t>Run 3</t>
   </si>
 </sst>
 </file>
@@ -670,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:J19"/>
+  <dimension ref="B2:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,13 +695,11 @@
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
@@ -713,7 +717,7 @@
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -723,17 +727,23 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
@@ -743,26 +753,32 @@
       <c r="D5" s="5">
         <v>10</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="4">
+        <v>10</v>
+      </c>
+      <c r="F5" s="5">
+        <v>10</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="5">
+      <c r="H5" s="5">
         <v>100</v>
       </c>
-      <c r="G5" s="4">
+      <c r="I5" s="4">
         <v>500</v>
       </c>
-      <c r="H5" s="18">
+      <c r="J5" s="18">
         <v>1000</v>
       </c>
-      <c r="I5" s="4">
+      <c r="K5" s="4">
         <v>10000</v>
       </c>
-      <c r="J5" s="19">
+      <c r="L5" s="19">
         <v>100000</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
@@ -772,10 +788,10 @@
       <c r="D6" s="31">
         <v>1000</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="6">
         <v>1000</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="31">
         <v>1000</v>
       </c>
       <c r="G6" s="8">
@@ -787,11 +803,17 @@
       <c r="I6" s="8">
         <v>1000</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="7">
+        <v>1000</v>
+      </c>
+      <c r="K6" s="8">
+        <v>1000</v>
+      </c>
+      <c r="L6" s="9">
         <v>955</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>4</v>
       </c>
@@ -801,26 +823,32 @@
       <c r="D7" s="8">
         <v>337</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="11">
+        <v>415</v>
+      </c>
+      <c r="F7" s="8">
+        <v>387</v>
+      </c>
+      <c r="G7" s="12">
         <v>966059</v>
       </c>
-      <c r="F7" s="8">
+      <c r="H7" s="8">
         <v>974.2</v>
       </c>
-      <c r="G7" s="12">
+      <c r="I7" s="12">
         <v>5075.5</v>
       </c>
-      <c r="H7" s="8">
+      <c r="J7" s="8">
         <v>9371.5</v>
       </c>
-      <c r="I7" s="12">
+      <c r="K7" s="12">
         <v>103811</v>
       </c>
-      <c r="J7" s="13">
+      <c r="L7" s="13">
         <v>1079720</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
@@ -830,26 +858,32 @@
       <c r="D8" s="7">
         <v>16</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="6">
+        <v>13</v>
+      </c>
+      <c r="F8" s="7">
+        <v>11</v>
+      </c>
+      <c r="G8" s="8">
         <v>8.6999999999999993</v>
       </c>
-      <c r="F8" s="7">
+      <c r="H8" s="7">
         <v>40.200000000000003</v>
       </c>
-      <c r="G8" s="8">
+      <c r="I8" s="8">
         <v>33.299999999999997</v>
       </c>
-      <c r="H8" s="7">
+      <c r="J8" s="7">
         <v>37.6</v>
       </c>
-      <c r="I8" s="8">
+      <c r="K8" s="8">
         <v>38</v>
       </c>
-      <c r="J8" s="9">
+      <c r="L8" s="9">
         <v>34.9</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>8</v>
       </c>
@@ -859,46 +893,52 @@
       <c r="D9" s="15">
         <v>49</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="14">
+        <v>60</v>
+      </c>
+      <c r="F9" s="15">
+        <v>64</v>
+      </c>
+      <c r="G9" s="16">
         <v>37431</v>
       </c>
-      <c r="F9" s="15">
+      <c r="H9" s="15">
         <v>19</v>
       </c>
-      <c r="G9" s="16">
+      <c r="I9" s="16">
         <v>21</v>
       </c>
-      <c r="H9" s="15">
+      <c r="J9" s="15">
         <v>18</v>
       </c>
-      <c r="I9" s="16">
+      <c r="K9" s="16">
         <v>19</v>
       </c>
-      <c r="J9" s="17">
+      <c r="L9" s="17">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>12</v>
+      </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
-    </row>
-    <row r="13" spans="2:10" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="13" spans="2:12" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B13" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E13" s="21" t="s">
         <v>1</v>
@@ -907,10 +947,21 @@
         <v>2</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="22" t="s">
         <v>3</v>
       </c>
@@ -921,27 +972,33 @@
         <v>10</v>
       </c>
       <c r="E16" s="23">
+        <v>10</v>
+      </c>
+      <c r="F16" s="23">
+        <v>10</v>
+      </c>
+      <c r="G16" s="23">
         <v>50</v>
       </c>
-      <c r="F16" s="23">
+      <c r="H16" s="23">
         <v>100</v>
       </c>
-      <c r="G16" s="23">
+      <c r="I16" s="23">
         <v>500</v>
       </c>
-      <c r="H16" s="23">
+      <c r="J16" s="23">
         <v>1000</v>
       </c>
-      <c r="I16" s="23">
+      <c r="K16" s="23">
         <v>10000</v>
       </c>
-      <c r="J16" s="24">
+      <c r="L16" s="24">
         <v>100000</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="26">
         <v>5</v>
@@ -950,25 +1007,31 @@
         <v>5</v>
       </c>
       <c r="E17" s="26">
+        <v>4</v>
+      </c>
+      <c r="F17" s="26">
+        <v>5</v>
+      </c>
+      <c r="G17" s="26">
         <v>2</v>
       </c>
-      <c r="F17" s="26">
+      <c r="H17" s="26">
         <v>4</v>
       </c>
-      <c r="G17" s="26">
+      <c r="I17" s="26">
         <v>5</v>
       </c>
-      <c r="H17" s="26">
+      <c r="J17" s="26">
         <v>3</v>
       </c>
-      <c r="I17" s="26">
+      <c r="K17" s="26">
         <v>3</v>
       </c>
-      <c r="J17" s="27">
+      <c r="L17" s="27">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="22" t="s">
         <v>4</v>
       </c>
@@ -979,25 +1042,31 @@
         <v>3007046</v>
       </c>
       <c r="E18" s="23">
+        <v>2425571</v>
+      </c>
+      <c r="F18" s="23">
+        <v>3040513</v>
+      </c>
+      <c r="G18" s="23">
         <v>4984</v>
       </c>
-      <c r="F18" s="23">
+      <c r="H18" s="23">
         <v>2878</v>
       </c>
-      <c r="G18" s="23">
+      <c r="I18" s="23">
         <v>2127</v>
       </c>
-      <c r="H18" s="23">
+      <c r="J18" s="23">
         <v>4820</v>
       </c>
-      <c r="I18" s="23">
+      <c r="K18" s="23">
         <v>2816</v>
       </c>
-      <c r="J18" s="24">
+      <c r="L18" s="24">
         <v>2420</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="28" t="s">
         <v>5</v>
       </c>
@@ -1008,21 +1077,27 @@
         <v>77</v>
       </c>
       <c r="E19" s="29">
+        <v>74</v>
+      </c>
+      <c r="F19" s="29">
+        <v>75</v>
+      </c>
+      <c r="G19" s="29">
         <v>1.2</v>
       </c>
-      <c r="F19" s="29">
+      <c r="H19" s="29">
         <v>4.0999999999999996</v>
       </c>
-      <c r="G19" s="29">
+      <c r="I19" s="29">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H19" s="29">
+      <c r="J19" s="29">
         <v>4.4000000000000004</v>
       </c>
-      <c r="I19" s="29">
+      <c r="K19" s="29">
         <v>3.9</v>
       </c>
-      <c r="J19" s="30">
+      <c r="L19" s="30">
         <v>1.1000000000000001</v>
       </c>
     </row>

</xml_diff>